<commit_message>
Major Changes, still in testing
Project is moving in a network documentation automation direction.
</commit_message>
<xml_diff>
--- a/dv-variables.xlsx
+++ b/dv-variables.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
   <si>
     <t>Variable</t>
   </si>
@@ -60,9 +60,6 @@
     <t>RoutingProtocol</t>
   </si>
   <si>
-    <t>this will record the results of the power budget and export it with the final dump</t>
-  </si>
-  <si>
     <t>ExportLocation</t>
   </si>
   <si>
@@ -72,15 +69,9 @@
     <t>Temperature</t>
   </si>
   <si>
-    <t>this will record the enviromental result and export it with the final dump</t>
-  </si>
-  <si>
     <t>DHCPSnooping</t>
   </si>
   <si>
-    <t>this will validate DHCP Snooping is enabled and export results with the final dump</t>
-  </si>
-  <si>
     <t>iPerfTest</t>
   </si>
   <si>
@@ -157,6 +148,39 @@
   </si>
   <si>
     <t>Configuration</t>
+  </si>
+  <si>
+    <t>CDPDiscovery</t>
+  </si>
+  <si>
+    <t>CDPSeed</t>
+  </si>
+  <si>
+    <t>Specify True/False for whether you want to do CDP discovery of devices</t>
+  </si>
+  <si>
+    <t>Specify the IP of a seed router</t>
+  </si>
+  <si>
+    <t>CDPDeviceType</t>
+  </si>
+  <si>
+    <t>Specify IOS/XE/NXOS</t>
+  </si>
+  <si>
+    <t>CDPDiscoveryDepth</t>
+  </si>
+  <si>
+    <t>Specify an integer (up to 10) for how deep you want to discover devices</t>
+  </si>
+  <si>
+    <t>Specify True/False, this will record the results of the power budget and export it with the final dump</t>
+  </si>
+  <si>
+    <t>Specify True/False, this will validate DHCP Snooping is enabled and export results with the final dump</t>
+  </si>
+  <si>
+    <t>Specify True/False, this will record the enviromental result and export it with the final dump</t>
   </si>
 </sst>
 </file>
@@ -209,11 +233,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -494,10 +519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -520,155 +545,191 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="3"/>
+      <c r="A5" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="2"/>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6" s="3"/>
-      <c r="C6" t="s">
-        <v>30</v>
+      <c r="A6" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B7" s="3"/>
-      <c r="C7" t="s">
-        <v>41</v>
+      <c r="A7" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="4" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="3"/>
-      <c r="C8" t="s">
-        <v>29</v>
+      <c r="A8" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="4" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" t="s">
-        <v>14</v>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="3"/>
+      <c r="C21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -682,7 +743,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -698,13 +759,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>8</v>

</xml_diff>